<commit_message>
Refactor cyclo rep alignment
</commit_message>
<xml_diff>
--- a/tabular/genus/cyclo_reference_feature_locations.xlsx
+++ b/tabular/genus/cyclo_reference_feature_locations.xlsx
@@ -5,16 +5,17 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3C960A-82A7-B44F-9E0D-D2E618B2D136}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BE71D0-154F-A346-A46D-C4A622F73903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="26220" windowHeight="14620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="31060" windowHeight="28340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>featureName</t>
   </si>
@@ -52,108 +53,6 @@
     <t>Mid-ORF</t>
   </si>
   <si>
-    <t>NC_001792</t>
-  </si>
-  <si>
-    <t>PCV-1</t>
-  </si>
-  <si>
-    <t>NC_005148</t>
-  </si>
-  <si>
-    <t>PCV-2</t>
-  </si>
-  <si>
-    <t>NC_031753</t>
-  </si>
-  <si>
-    <t>PCV-3</t>
-  </si>
-  <si>
-    <t>NC_020904</t>
-  </si>
-  <si>
-    <t>CfCV</t>
-  </si>
-  <si>
-    <t>NC_023885</t>
-  </si>
-  <si>
-    <t>MiCV</t>
-  </si>
-  <si>
-    <t>NC_028045</t>
-  </si>
-  <si>
-    <t>TbCV</t>
-  </si>
-  <si>
-    <t>NC_001944</t>
-  </si>
-  <si>
-    <t>BFDV</t>
-  </si>
-  <si>
-    <t>NC_003410</t>
-  </si>
-  <si>
-    <t>CaCV</t>
-  </si>
-  <si>
-    <t>NC_008033</t>
-  </si>
-  <si>
-    <t>SvCV</t>
-  </si>
-  <si>
-    <t>NC_008375</t>
-  </si>
-  <si>
-    <t>RaCV</t>
-  </si>
-  <si>
-    <t>NC_008521</t>
-  </si>
-  <si>
-    <t>GuCV</t>
-  </si>
-  <si>
-    <t>NC_008522</t>
-  </si>
-  <si>
-    <t>FiCV</t>
-  </si>
-  <si>
-    <t>NC_007220</t>
-  </si>
-  <si>
-    <t>DuCV</t>
-  </si>
-  <si>
-    <t>NC_025247</t>
-  </si>
-  <si>
-    <t>SwCV</t>
-  </si>
-  <si>
-    <t>NC_026945</t>
-  </si>
-  <si>
-    <t>ZfCV</t>
-  </si>
-  <si>
-    <t>NC_015399</t>
-  </si>
-  <si>
-    <t>BarbCV</t>
-  </si>
-  <si>
-    <t>NC_025246</t>
-  </si>
-  <si>
-    <t>SgCV</t>
-  </si>
-  <si>
     <t>Rep</t>
   </si>
   <si>
@@ -169,13 +68,7 @@
     <t>gp2</t>
   </si>
   <si>
-    <t>KJ831064</t>
-  </si>
-  <si>
     <t>KM382270</t>
-  </si>
-  <si>
-    <t>HuACyV-1</t>
   </si>
   <si>
     <t>BatACyV-10</t>
@@ -196,22 +89,7 @@
     <t>Cyclovirus</t>
   </si>
   <si>
-    <t>Circovirus</t>
-  </si>
-  <si>
-    <t>5UTR</t>
-  </si>
-  <si>
-    <t>3UTR</t>
-  </si>
-  <si>
     <t>Cap</t>
-  </si>
-  <si>
-    <t>ORFV2</t>
-  </si>
-  <si>
-    <t>ORFC2</t>
   </si>
   <si>
     <t>gp3</t>
@@ -232,76 +110,10 @@
     <t>AHEaCV-14</t>
   </si>
   <si>
-    <t>NC_002361</t>
-  </si>
-  <si>
-    <t>CoCV</t>
-  </si>
-  <si>
     <t>NC_024700</t>
   </si>
   <si>
     <t>Feline cyclovirus</t>
-  </si>
-  <si>
-    <t>StCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_MASTER_PCV-1</t>
-  </si>
-  <si>
-    <t>REF_Circo_BFDV</t>
-  </si>
-  <si>
-    <t>REF_Circo_CaCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_PCV-2</t>
-  </si>
-  <si>
-    <t>REF_Circo_StCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_DuCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_SvCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_RaCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_GuCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_CoCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_FiCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_BarbCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_CfCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_MiCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_SgCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_SwCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_ZfCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_TbCV</t>
-  </si>
-  <si>
-    <t>REF_Circo_PCV-3</t>
   </si>
   <si>
     <t>REF_Cyclo_BatACyV-10</t>
@@ -314,9 +126,6 @@
   </si>
   <si>
     <t>REF_CRESS1_AHEaCV-14</t>
-  </si>
-  <si>
-    <t>REF_Cyclo_MASTER_HuACyV-1</t>
   </si>
   <si>
     <t>whole_genome</t>
@@ -338,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,12 +202,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -406,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,18 +248,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2DCDB"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDAEEF3"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -2540,7 +2331,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2562,17 +2353,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2061">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -4972,10 +4759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1540"/>
+  <dimension ref="A1:G1470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69:G71"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4992,16 +4779,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>0</v>
@@ -5014,2079 +4801,661 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>55</v>
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
       </c>
       <c r="G2" s="6">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="F3" s="6">
+        <v>208</v>
+      </c>
+      <c r="G3" s="6">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1005</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="6">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="G5" s="6">
+        <v>2904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="6">
-        <v>55</v>
-      </c>
-      <c r="G4" s="6">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1038</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="F6" s="6">
-        <v>1731</v>
-      </c>
-      <c r="G6" s="17">
-        <v>1758</v>
+        <v>606</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1583</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="F7" s="6">
-        <v>1</v>
+        <v>1741</v>
       </c>
       <c r="G7" s="6">
-        <v>1993</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="F8" s="6">
-        <v>108</v>
+        <v>2329</v>
       </c>
       <c r="G8" s="6">
-        <v>1007</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="F9" s="6">
-        <v>550</v>
+        <v>1</v>
       </c>
       <c r="G9" s="6">
-        <v>1026</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1240</v>
-      </c>
-      <c r="G10" s="6">
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="F11" s="6">
-        <v>1</v>
+        <v>827</v>
       </c>
       <c r="G11" s="6">
-        <v>1952</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="6">
-        <v>32</v>
-      </c>
-      <c r="G12" s="6">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1154</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1906</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="6">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="6">
-        <v>51</v>
-      </c>
-      <c r="G15" s="6">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="6">
-        <v>357</v>
-      </c>
-      <c r="G16" s="6">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1034</v>
-      </c>
-      <c r="G17" s="6">
-        <v>1735</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1</v>
-      </c>
-      <c r="G18" s="6">
-        <v>2063</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="6">
-        <v>37</v>
-      </c>
-      <c r="G19" s="6">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="6">
-        <v>834</v>
-      </c>
-      <c r="G20" s="6">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1190</v>
-      </c>
-      <c r="G21" s="6">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="6">
-        <v>48</v>
-      </c>
-      <c r="G23" s="6">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="6">
-        <v>423</v>
-      </c>
-      <c r="G24" s="6">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="6">
-        <v>1155</v>
-      </c>
-      <c r="G25" s="6">
-        <v>1928</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="6">
-        <v>1</v>
-      </c>
-      <c r="G26" s="6">
-        <v>2063</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="6">
-        <v>37</v>
-      </c>
-      <c r="G27" s="6">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="6">
-        <v>1190</v>
-      </c>
-      <c r="G28" s="6">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="6">
-        <v>1</v>
-      </c>
-      <c r="G29" s="6">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" s="6">
-        <v>36</v>
-      </c>
-      <c r="G30" s="6">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1116</v>
-      </c>
-      <c r="G31" s="6">
-        <v>1844</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="6">
-        <v>2035</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="6">
-        <v>100</v>
-      </c>
-      <c r="G33" s="6">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="6">
-        <v>790</v>
-      </c>
-      <c r="G34" s="6">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F35" s="6">
-        <v>1190</v>
-      </c>
-      <c r="G35" s="6">
-        <v>1927</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F36" s="6">
-        <v>1</v>
-      </c>
-      <c r="G36" s="6">
-        <v>2037</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" s="6">
-        <v>41</v>
-      </c>
-      <c r="G37" s="6">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="6">
-        <v>410</v>
-      </c>
-      <c r="G38" s="6">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" s="6">
-        <v>1166</v>
-      </c>
-      <c r="G39" s="6">
-        <v>1987</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="6">
-        <v>1</v>
-      </c>
-      <c r="G40" s="6">
-        <v>1962</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="6">
-        <v>29</v>
-      </c>
-      <c r="G41" s="6">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F42" s="6">
-        <v>614</v>
-      </c>
-      <c r="G42" s="6">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F43" s="6">
-        <v>1</v>
-      </c>
-      <c r="G43" s="6">
-        <v>1957</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="6">
-        <v>48</v>
-      </c>
-      <c r="G44" s="6">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F45" s="6">
-        <v>1261</v>
-      </c>
-      <c r="G45" s="6">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F46" s="6">
-        <v>1</v>
-      </c>
-      <c r="G46" s="6">
-        <v>2063</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="6">
-        <v>1</v>
-      </c>
-      <c r="G47" s="6">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F48" s="6">
-        <v>1116</v>
-      </c>
-      <c r="G48" s="6">
-        <v>1928</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F49" s="6">
-        <v>1</v>
-      </c>
-      <c r="G49" s="6">
-        <v>1753</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" s="6">
-        <v>36</v>
-      </c>
-      <c r="G50" s="6">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F51" s="6">
-        <v>1020</v>
-      </c>
-      <c r="G51" s="6">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F52" s="6">
-        <v>1</v>
-      </c>
-      <c r="G52" s="6">
-        <v>1966</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="6">
-        <v>251</v>
-      </c>
-      <c r="G53" s="6">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F54" s="6">
-        <v>1251</v>
-      </c>
-      <c r="G54" s="6">
-        <v>1934</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="6">
-        <v>1</v>
-      </c>
-      <c r="G55" s="6">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F56" s="6">
-        <v>48</v>
-      </c>
-      <c r="G56" s="6">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F57" s="6">
-        <v>968</v>
-      </c>
-      <c r="G57" s="6">
-        <v>1723</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="6">
-        <v>1</v>
-      </c>
-      <c r="G58" s="6">
-        <v>1982</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F59" s="6">
-        <v>29</v>
-      </c>
-      <c r="G59" s="6">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F60" s="6">
-        <v>1233</v>
-      </c>
-      <c r="G60" s="6">
-        <v>1967</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F61" s="6">
-        <v>1289</v>
-      </c>
-      <c r="G61" s="6">
-        <v>1720</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F62" s="6">
-        <v>1233</v>
-      </c>
-      <c r="G62" s="6">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="6">
-        <v>1</v>
-      </c>
-      <c r="G63" s="6">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F64" s="6">
-        <v>8</v>
-      </c>
-      <c r="G64" s="6">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F65" s="6">
-        <v>1055</v>
-      </c>
-      <c r="G65" s="6">
-        <v>1711</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F66" s="6">
-        <v>1</v>
-      </c>
-      <c r="G66" s="6">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F67" s="6">
-        <v>216</v>
-      </c>
-      <c r="G67" s="6">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F68" s="6">
-        <v>1336</v>
-      </c>
-      <c r="G68" s="6">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F69" s="6">
-        <v>1</v>
-      </c>
-      <c r="G69" s="6">
-        <v>1710</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F70" s="6">
-        <v>26</v>
-      </c>
-      <c r="G70" s="6">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F71" s="6">
-        <v>836</v>
-      </c>
-      <c r="G71" s="6">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F72" s="6">
-        <v>1</v>
-      </c>
-      <c r="G72" s="6">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F73" s="6">
-        <v>208</v>
-      </c>
-      <c r="G73" s="6">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F74" s="6">
-        <v>1005</v>
-      </c>
-      <c r="G74" s="6">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C75" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F75" s="6">
-        <v>1</v>
-      </c>
-      <c r="G75" s="6">
-        <v>2904</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F76" s="6">
-        <v>606</v>
-      </c>
-      <c r="G76" s="6">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C77" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F77" s="6">
-        <v>1741</v>
-      </c>
-      <c r="G77" s="6">
-        <v>2313</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C78" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F78" s="6">
-        <v>2329</v>
-      </c>
-      <c r="G78" s="6">
-        <v>2904</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C79" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F79" s="6">
-        <v>1</v>
-      </c>
-      <c r="G79" s="6">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C80" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F80" s="6">
-        <v>1</v>
-      </c>
-      <c r="G80" s="6">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C81" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F81" s="6">
-        <v>827</v>
-      </c>
-      <c r="G81" s="6">
         <v>1498</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F82" s="6">
-        <v>1</v>
-      </c>
-      <c r="G82" s="6">
-        <v>2212</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F83">
-        <v>153</v>
-      </c>
-      <c r="G83">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F84">
-        <v>1042</v>
-      </c>
-      <c r="G84">
-        <v>2145</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>65</v>
-      </c>
-      <c r="B85" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F85" s="6">
-        <v>1</v>
-      </c>
-      <c r="G85" s="6">
-        <v>2255</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>65</v>
-      </c>
-      <c r="B86" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C86" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F86" s="6">
-        <v>79</v>
-      </c>
-      <c r="G86" s="6">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>65</v>
-      </c>
-      <c r="B87" t="s">
-        <v>66</v>
-      </c>
-      <c r="C87" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F87" s="6">
-        <v>1139</v>
-      </c>
-      <c r="G87" s="6">
-        <v>2086</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>97</v>
-      </c>
-      <c r="B88" t="s">
-        <v>99</v>
-      </c>
-      <c r="C88" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D88" t="s">
-        <v>98</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F88" s="6">
-        <v>1</v>
-      </c>
-      <c r="G88">
-        <v>2926</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>97</v>
-      </c>
-      <c r="B89" t="s">
-        <v>99</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D89" t="s">
-        <v>98</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F89" s="6">
-        <v>1</v>
-      </c>
-      <c r="G89">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>97</v>
-      </c>
-      <c r="B90" t="s">
-        <v>99</v>
-      </c>
-      <c r="C90" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D90" t="s">
-        <v>98</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F90" s="6">
-        <v>350</v>
-      </c>
-      <c r="G90">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>97</v>
-      </c>
-      <c r="B91" t="s">
-        <v>99</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D91" t="s">
-        <v>98</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F91" s="6">
-        <v>1366</v>
-      </c>
-      <c r="G91">
-        <v>2874</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E94" s="8"/>
-    </row>
-    <row r="100" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="5:5" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="8"/>
+    </row>
+    <row r="30" spans="5:5" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="9"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="9"/>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="9"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="9"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="9"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="9"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="9"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="9"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="9"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="9"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="9"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="9"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="9"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="9"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="9"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="9"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="9"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="9"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="9"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="9"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="9"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="9"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="9"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="9"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="9"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="9"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="9"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="9"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="9"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="9"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="9"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="9"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="9"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="9"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="9"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="9"/>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="9"/>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="9"/>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="9"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="9"/>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="9"/>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="9"/>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="9"/>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="9"/>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="9"/>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="9"/>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="9"/>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="9"/>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="9"/>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="9"/>
+    </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -7117,722 +5486,385 @@
       <c r="D112" s="2"/>
       <c r="E112" s="9"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
       <c r="E113" s="9"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="9"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="9"/>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
       <c r="E116" s="9"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="9"/>
-      <c r="G117" s="2"/>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="9"/>
-      <c r="G118" s="2"/>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="9"/>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="9"/>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="9"/>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="9"/>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="9"/>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="9"/>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="9"/>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="9"/>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="9"/>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="9"/>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="9"/>
-    </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="9"/>
-    </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="9"/>
-    </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="9"/>
-    </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="9"/>
-    </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="9"/>
-    </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="9"/>
-    </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="2"/>
-      <c r="E136" s="9"/>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="9"/>
-    </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="9"/>
-    </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="2"/>
-      <c r="E139" s="9"/>
-      <c r="F139" s="1"/>
-    </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="9"/>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="9"/>
-    </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="9"/>
-    </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="9"/>
-    </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="9"/>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-      <c r="E146" s="9"/>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="9"/>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="9"/>
-    </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="9"/>
-    </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="9"/>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="9"/>
-    </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="9"/>
-    </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="9"/>
-    </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="9"/>
-    </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="9"/>
-    </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="9"/>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
-      <c r="E157" s="9"/>
-    </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="9"/>
-    </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="9"/>
-    </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="9"/>
-    </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
-      <c r="E161" s="9"/>
-    </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="9"/>
-    </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
-      <c r="E163" s="9"/>
-    </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="9"/>
-    </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
-      <c r="D165" s="2"/>
-      <c r="E165" s="9"/>
-    </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="9"/>
-    </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="9"/>
-    </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
-      <c r="D168" s="2"/>
-      <c r="E168" s="9"/>
-    </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
-      <c r="D169" s="2"/>
-      <c r="E169" s="9"/>
-    </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-      <c r="D170" s="2"/>
-      <c r="E170" s="9"/>
-    </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
-      <c r="D171" s="2"/>
-      <c r="E171" s="9"/>
-    </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
-      <c r="D172" s="2"/>
-      <c r="E172" s="9"/>
-    </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
-      <c r="D173" s="2"/>
-      <c r="E173" s="9"/>
-    </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="2"/>
-      <c r="E174" s="9"/>
-    </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
-      <c r="D175" s="2"/>
-      <c r="E175" s="9"/>
-    </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
-      <c r="D176" s="2"/>
-      <c r="E176" s="9"/>
-    </row>
-    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
-      <c r="D177" s="2"/>
-      <c r="E177" s="9"/>
-    </row>
-    <row r="178" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
-      <c r="D178" s="2"/>
-      <c r="E178" s="9"/>
-    </row>
-    <row r="179" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
-      <c r="D179" s="2"/>
-      <c r="E179" s="9"/>
-    </row>
-    <row r="180" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
-      <c r="D180" s="2"/>
-      <c r="E180" s="9"/>
-    </row>
-    <row r="181" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
-      <c r="D181" s="2"/>
-      <c r="E181" s="9"/>
-    </row>
-    <row r="182" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
-      <c r="D182" s="2"/>
-      <c r="E182" s="9"/>
-    </row>
-    <row r="183" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
-      <c r="D183" s="2"/>
-      <c r="E183" s="9"/>
-    </row>
-    <row r="184" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
-      <c r="D184" s="2"/>
-      <c r="E184" s="9"/>
-    </row>
-    <row r="185" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-      <c r="D185" s="2"/>
-      <c r="E185" s="9"/>
-    </row>
-    <row r="186" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
-      <c r="D186" s="2"/>
-      <c r="E186" s="9"/>
-    </row>
-    <row r="262" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B262" s="2"/>
-      <c r="C262" s="2"/>
-      <c r="D262" s="2"/>
-      <c r="E262" s="9"/>
-    </row>
-    <row r="263" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B263" s="2"/>
-      <c r="C263" s="2"/>
-      <c r="D263" s="2"/>
-      <c r="E263" s="9"/>
-    </row>
-    <row r="264" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B264" s="2"/>
-      <c r="C264" s="2"/>
-      <c r="D264" s="2"/>
-      <c r="E264" s="9"/>
-    </row>
-    <row r="265" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B265" s="2"/>
-      <c r="C265" s="2"/>
-      <c r="D265" s="2"/>
-      <c r="E265" s="9"/>
-    </row>
-    <row r="266" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B266" s="2"/>
-      <c r="C266" s="2"/>
-      <c r="D266" s="2"/>
-      <c r="E266" s="9"/>
-    </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B267" s="2"/>
-      <c r="C267" s="2"/>
-      <c r="D267" s="2"/>
-      <c r="E267" s="9"/>
-    </row>
-    <row r="268" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B268" s="2"/>
-      <c r="C268" s="2"/>
-      <c r="D268" s="2"/>
-      <c r="E268" s="9"/>
-    </row>
-    <row r="269" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B269" s="2"/>
-      <c r="C269" s="2"/>
-      <c r="D269" s="2"/>
-      <c r="E269" s="9"/>
-    </row>
-    <row r="270" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B270" s="2"/>
-      <c r="C270" s="2"/>
-      <c r="D270" s="2"/>
-      <c r="E270" s="9"/>
-    </row>
-    <row r="271" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B271" s="2"/>
-      <c r="C271" s="2"/>
-      <c r="D271" s="2"/>
-      <c r="E271" s="9"/>
-    </row>
-    <row r="272" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B272" s="2"/>
-      <c r="C272" s="2"/>
-      <c r="D272" s="2"/>
-      <c r="E272" s="9"/>
-    </row>
-    <row r="273" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B273" s="2"/>
-      <c r="C273" s="2"/>
-      <c r="D273" s="2"/>
-      <c r="E273" s="9"/>
-    </row>
-    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B274" s="2"/>
-      <c r="C274" s="2"/>
-      <c r="D274" s="2"/>
-      <c r="E274" s="9"/>
-    </row>
-    <row r="275" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B275" s="2"/>
-      <c r="C275" s="2"/>
-      <c r="D275" s="2"/>
-      <c r="E275" s="9"/>
-    </row>
-    <row r="276" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B276" s="2"/>
-      <c r="C276" s="2"/>
-      <c r="D276" s="2"/>
-      <c r="E276" s="9"/>
-    </row>
-    <row r="277" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B277" s="2"/>
-      <c r="C277" s="2"/>
-      <c r="D277" s="2"/>
-      <c r="E277" s="9"/>
-    </row>
-    <row r="278" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B278" s="2"/>
-      <c r="C278" s="2"/>
-      <c r="D278" s="2"/>
-      <c r="E278" s="9"/>
-    </row>
-    <row r="279" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B279" s="2"/>
-      <c r="C279" s="2"/>
-      <c r="D279" s="2"/>
-      <c r="E279" s="9"/>
-    </row>
-    <row r="280" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B280" s="2"/>
-      <c r="C280" s="2"/>
-      <c r="D280" s="2"/>
-      <c r="E280" s="9"/>
-    </row>
-    <row r="281" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B281" s="2"/>
-      <c r="C281" s="2"/>
-      <c r="D281" s="2"/>
-      <c r="E281" s="9"/>
-    </row>
-    <row r="282" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B282" s="2"/>
-      <c r="C282" s="2"/>
-      <c r="D282" s="2"/>
-      <c r="E282" s="9"/>
-    </row>
-    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B283" s="2"/>
-      <c r="C283" s="2"/>
-      <c r="D283" s="2"/>
-      <c r="E283" s="9"/>
-    </row>
-    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B284" s="2"/>
-      <c r="C284" s="2"/>
-      <c r="D284" s="2"/>
-      <c r="E284" s="9"/>
-    </row>
-    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B285" s="2"/>
-      <c r="C285" s="2"/>
-      <c r="D285" s="2"/>
-      <c r="E285" s="9"/>
-    </row>
-    <row r="286" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B286" s="2"/>
-      <c r="C286" s="2"/>
-      <c r="D286" s="2"/>
-    </row>
-    <row r="287" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B287" s="2"/>
-      <c r="C287" s="2"/>
-      <c r="D287" s="2"/>
-      <c r="E287" s="9"/>
-    </row>
-    <row r="288" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B288" s="2"/>
-      <c r="C288" s="2"/>
-      <c r="D288" s="2"/>
-      <c r="E288" s="9"/>
-    </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B289" s="2"/>
-      <c r="C289" s="2"/>
-      <c r="D289" s="2"/>
-      <c r="E289" s="9"/>
-    </row>
-    <row r="290" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B290" s="2"/>
-      <c r="C290" s="2"/>
-      <c r="D290" s="2"/>
-      <c r="E290" s="9"/>
-    </row>
-    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B291" s="2"/>
-      <c r="C291" s="2"/>
-      <c r="D291" s="2"/>
-      <c r="E291" s="9"/>
-    </row>
-    <row r="292" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B292" s="2"/>
-      <c r="C292" s="2"/>
-      <c r="D292" s="2"/>
-      <c r="E292" s="9"/>
-    </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B293" s="2"/>
-      <c r="C293" s="2"/>
-      <c r="D293" s="2"/>
-      <c r="E293" s="9"/>
-    </row>
-    <row r="976" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F976" s="2"/>
-    </row>
-    <row r="1112" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1112" s="2"/>
-      <c r="C1112" s="2"/>
-      <c r="D1112" s="2"/>
-    </row>
-    <row r="1113" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1113" s="2"/>
-      <c r="C1113" s="2"/>
-      <c r="D1113" s="2"/>
-    </row>
-    <row r="1238" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1238" s="2"/>
-      <c r="C1238" s="2"/>
-      <c r="D1238" s="2"/>
-    </row>
-    <row r="1239" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1239" s="2"/>
-      <c r="C1239" s="2"/>
-      <c r="D1239" s="2"/>
-    </row>
-    <row r="1240" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1240" s="2"/>
-      <c r="C1240" s="2"/>
-      <c r="D1240" s="2"/>
-    </row>
-    <row r="1241" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1241" s="2"/>
-      <c r="C1241" s="2"/>
-      <c r="D1241" s="2"/>
-    </row>
-    <row r="1242" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1242" s="2"/>
-      <c r="C1242" s="2"/>
-      <c r="D1242" s="2"/>
-    </row>
-    <row r="1243" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1243" s="2"/>
-      <c r="C1243" s="2"/>
-      <c r="D1243" s="2"/>
-    </row>
-    <row r="1288" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F1288" s="2"/>
-      <c r="G1288" s="2"/>
-    </row>
-    <row r="1289" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F1289" s="2"/>
-      <c r="G1289" s="2"/>
-    </row>
-    <row r="1290" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F1290" s="2"/>
-      <c r="G1290" s="2"/>
-    </row>
-    <row r="1292" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1292" s="2"/>
-      <c r="C1292" s="2"/>
-      <c r="D1292" s="2"/>
-    </row>
-    <row r="1293" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1293" s="2"/>
-      <c r="C1293" s="2"/>
-      <c r="D1293" s="2"/>
-    </row>
-    <row r="1294" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1294" s="2"/>
-      <c r="C1294" s="2"/>
-      <c r="D1294" s="2"/>
-    </row>
-    <row r="1295" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1295" s="2"/>
-      <c r="C1295" s="2"/>
-      <c r="D1295" s="2"/>
-    </row>
-    <row r="1296" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1296" s="2"/>
-      <c r="C1296" s="2"/>
-      <c r="D1296" s="2"/>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2"/>
+      <c r="E192" s="9"/>
+    </row>
+    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
+      <c r="D193" s="2"/>
+      <c r="E193" s="9"/>
+    </row>
+    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B194" s="2"/>
+      <c r="C194" s="2"/>
+      <c r="D194" s="2"/>
+      <c r="E194" s="9"/>
+    </row>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B195" s="2"/>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
+      <c r="E195" s="9"/>
+    </row>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B196" s="2"/>
+      <c r="C196" s="2"/>
+      <c r="D196" s="2"/>
+      <c r="E196" s="9"/>
+    </row>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B197" s="2"/>
+      <c r="C197" s="2"/>
+      <c r="D197" s="2"/>
+      <c r="E197" s="9"/>
+    </row>
+    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B198" s="2"/>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2"/>
+      <c r="E198" s="9"/>
+    </row>
+    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B199" s="2"/>
+      <c r="C199" s="2"/>
+      <c r="D199" s="2"/>
+      <c r="E199" s="9"/>
+    </row>
+    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B200" s="2"/>
+      <c r="C200" s="2"/>
+      <c r="D200" s="2"/>
+      <c r="E200" s="9"/>
+    </row>
+    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B201" s="2"/>
+      <c r="C201" s="2"/>
+      <c r="D201" s="2"/>
+      <c r="E201" s="9"/>
+    </row>
+    <row r="202" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B202" s="2"/>
+      <c r="C202" s="2"/>
+      <c r="D202" s="2"/>
+      <c r="E202" s="9"/>
+    </row>
+    <row r="203" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B203" s="2"/>
+      <c r="C203" s="2"/>
+      <c r="D203" s="2"/>
+      <c r="E203" s="9"/>
+    </row>
+    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B204" s="2"/>
+      <c r="C204" s="2"/>
+      <c r="D204" s="2"/>
+      <c r="E204" s="9"/>
+    </row>
+    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
+      <c r="D205" s="2"/>
+      <c r="E205" s="9"/>
+    </row>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
+      <c r="D206" s="2"/>
+      <c r="E206" s="9"/>
+    </row>
+    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
+      <c r="D207" s="2"/>
+      <c r="E207" s="9"/>
+    </row>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B208" s="2"/>
+      <c r="C208" s="2"/>
+      <c r="D208" s="2"/>
+      <c r="E208" s="9"/>
+    </row>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B209" s="2"/>
+      <c r="C209" s="2"/>
+      <c r="D209" s="2"/>
+      <c r="E209" s="9"/>
+    </row>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
+      <c r="D210" s="2"/>
+      <c r="E210" s="9"/>
+    </row>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
+      <c r="E211" s="9"/>
+    </row>
+    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
+      <c r="E212" s="9"/>
+    </row>
+    <row r="213" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B213" s="2"/>
+      <c r="C213" s="2"/>
+      <c r="D213" s="2"/>
+      <c r="E213" s="9"/>
+    </row>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B214" s="2"/>
+      <c r="C214" s="2"/>
+      <c r="D214" s="2"/>
+      <c r="E214" s="9"/>
+    </row>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
+      <c r="D215" s="2"/>
+      <c r="E215" s="9"/>
+    </row>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
+      <c r="D216" s="2"/>
+    </row>
+    <row r="217" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+      <c r="E217" s="9"/>
+    </row>
+    <row r="218" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B218" s="2"/>
+      <c r="C218" s="2"/>
+      <c r="D218" s="2"/>
+      <c r="E218" s="9"/>
+    </row>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B219" s="2"/>
+      <c r="C219" s="2"/>
+      <c r="D219" s="2"/>
+      <c r="E219" s="9"/>
+    </row>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B220" s="2"/>
+      <c r="C220" s="2"/>
+      <c r="D220" s="2"/>
+      <c r="E220" s="9"/>
+    </row>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B221" s="2"/>
+      <c r="C221" s="2"/>
+      <c r="D221" s="2"/>
+      <c r="E221" s="9"/>
+    </row>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B222" s="2"/>
+      <c r="C222" s="2"/>
+      <c r="D222" s="2"/>
+      <c r="E222" s="9"/>
+    </row>
+    <row r="223" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B223" s="2"/>
+      <c r="C223" s="2"/>
+      <c r="D223" s="2"/>
+      <c r="E223" s="9"/>
+    </row>
+    <row r="906" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F906" s="2"/>
+    </row>
+    <row r="1042" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1042" s="2"/>
+      <c r="C1042" s="2"/>
+      <c r="D1042" s="2"/>
+    </row>
+    <row r="1043" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1043" s="2"/>
+      <c r="C1043" s="2"/>
+      <c r="D1043" s="2"/>
+    </row>
+    <row r="1168" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1168" s="2"/>
+      <c r="C1168" s="2"/>
+      <c r="D1168" s="2"/>
+    </row>
+    <row r="1169" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1169" s="2"/>
+      <c r="C1169" s="2"/>
+      <c r="D1169" s="2"/>
+    </row>
+    <row r="1170" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1170" s="2"/>
+      <c r="C1170" s="2"/>
+      <c r="D1170" s="2"/>
+    </row>
+    <row r="1171" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1171" s="2"/>
+      <c r="C1171" s="2"/>
+      <c r="D1171" s="2"/>
+    </row>
+    <row r="1172" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1172" s="2"/>
+      <c r="C1172" s="2"/>
+      <c r="D1172" s="2"/>
+    </row>
+    <row r="1173" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1173" s="2"/>
+      <c r="C1173" s="2"/>
+      <c r="D1173" s="2"/>
+    </row>
+    <row r="1218" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F1218" s="2"/>
+      <c r="G1218" s="2"/>
+    </row>
+    <row r="1219" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F1219" s="2"/>
+      <c r="G1219" s="2"/>
+    </row>
+    <row r="1220" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F1220" s="2"/>
+      <c r="G1220" s="2"/>
+    </row>
+    <row r="1222" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1222" s="2"/>
+      <c r="C1222" s="2"/>
+      <c r="D1222" s="2"/>
+    </row>
+    <row r="1223" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1223" s="2"/>
+      <c r="C1223" s="2"/>
+      <c r="D1223" s="2"/>
+    </row>
+    <row r="1224" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1224" s="2"/>
+      <c r="C1224" s="2"/>
+      <c r="D1224" s="2"/>
+    </row>
+    <row r="1225" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1225" s="2"/>
+      <c r="C1225" s="2"/>
+      <c r="D1225" s="2"/>
+    </row>
+    <row r="1226" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1226" s="2"/>
+      <c r="C1226" s="2"/>
+      <c r="D1226" s="2"/>
+    </row>
+    <row r="1245" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1245" s="2"/>
+      <c r="C1245" s="2"/>
+      <c r="D1245" s="2"/>
+    </row>
+    <row r="1246" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1246" s="2"/>
+      <c r="C1246" s="2"/>
+      <c r="D1246" s="2"/>
+    </row>
+    <row r="1247" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1247" s="2"/>
+      <c r="C1247" s="2"/>
+      <c r="D1247" s="2"/>
+    </row>
+    <row r="1248" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1248" s="2"/>
+      <c r="C1248" s="2"/>
+      <c r="D1248" s="2"/>
+    </row>
+    <row r="1249" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1249" s="2"/>
+      <c r="C1249" s="2"/>
+      <c r="D1249" s="2"/>
+    </row>
+    <row r="1250" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1250" s="2"/>
+      <c r="C1250" s="2"/>
+      <c r="D1250" s="2"/>
+    </row>
+    <row r="1251" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1251" s="2"/>
+      <c r="C1251" s="2"/>
+      <c r="D1251" s="2"/>
+    </row>
+    <row r="1253" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1253" s="2"/>
+      <c r="C1253" s="2"/>
+      <c r="D1253" s="2"/>
+    </row>
+    <row r="1254" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1254" s="2"/>
+      <c r="C1254" s="2"/>
+      <c r="D1254" s="2"/>
+    </row>
+    <row r="1255" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1255" s="2"/>
+      <c r="C1255" s="2"/>
+      <c r="D1255" s="2"/>
+    </row>
+    <row r="1256" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1256" s="2"/>
+      <c r="C1256" s="2"/>
+      <c r="D1256" s="2"/>
+    </row>
+    <row r="1257" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1257" s="2"/>
+      <c r="C1257" s="2"/>
+      <c r="D1257" s="2"/>
+    </row>
+    <row r="1258" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1258" s="2"/>
+      <c r="C1258" s="2"/>
+      <c r="D1258" s="2"/>
+    </row>
+    <row r="1310" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1310" s="2"/>
+      <c r="C1310" s="2"/>
+      <c r="D1310" s="2"/>
+    </row>
+    <row r="1311" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1311" s="2"/>
+      <c r="C1311" s="2"/>
+      <c r="D1311" s="2"/>
+    </row>
+    <row r="1312" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1312" s="2"/>
+      <c r="C1312" s="2"/>
+      <c r="D1312" s="2"/>
+    </row>
+    <row r="1313" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1313" s="2"/>
+      <c r="C1313" s="2"/>
+      <c r="D1313" s="2"/>
     </row>
     <row r="1315" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1315" s="2"/>
@@ -7854,169 +5886,84 @@
       <c r="C1318" s="2"/>
       <c r="D1318" s="2"/>
     </row>
-    <row r="1319" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1319" s="2"/>
-      <c r="C1319" s="2"/>
-      <c r="D1319" s="2"/>
-    </row>
-    <row r="1320" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1320" s="2"/>
-      <c r="C1320" s="2"/>
-      <c r="D1320" s="2"/>
-    </row>
-    <row r="1321" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1321" s="2"/>
-      <c r="C1321" s="2"/>
-      <c r="D1321" s="2"/>
-    </row>
-    <row r="1323" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1323" s="2"/>
-      <c r="C1323" s="2"/>
-      <c r="D1323" s="2"/>
-    </row>
-    <row r="1324" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1324" s="2"/>
-      <c r="C1324" s="2"/>
-      <c r="D1324" s="2"/>
-    </row>
-    <row r="1325" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1325" s="2"/>
-      <c r="C1325" s="2"/>
-      <c r="D1325" s="2"/>
-    </row>
-    <row r="1326" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1326" s="2"/>
-      <c r="C1326" s="2"/>
-      <c r="D1326" s="2"/>
-    </row>
-    <row r="1327" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1327" s="2"/>
-      <c r="C1327" s="2"/>
-      <c r="D1327" s="2"/>
-    </row>
-    <row r="1328" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1328" s="2"/>
-      <c r="C1328" s="2"/>
-      <c r="D1328" s="2"/>
-    </row>
-    <row r="1380" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1380" s="2"/>
-      <c r="C1380" s="2"/>
-      <c r="D1380" s="2"/>
-    </row>
-    <row r="1381" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1381" s="2"/>
-      <c r="C1381" s="2"/>
-      <c r="D1381" s="2"/>
-    </row>
-    <row r="1382" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1382" s="2"/>
-      <c r="C1382" s="2"/>
-      <c r="D1382" s="2"/>
-    </row>
-    <row r="1383" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1383" s="2"/>
-      <c r="C1383" s="2"/>
-      <c r="D1383" s="2"/>
-    </row>
-    <row r="1385" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1385" s="2"/>
-      <c r="C1385" s="2"/>
-      <c r="D1385" s="2"/>
-    </row>
-    <row r="1386" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1386" s="2"/>
-      <c r="C1386" s="2"/>
-      <c r="D1386" s="2"/>
-    </row>
-    <row r="1387" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1387" s="2"/>
-      <c r="C1387" s="2"/>
-      <c r="D1387" s="2"/>
-    </row>
-    <row r="1388" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1388" s="2"/>
-      <c r="C1388" s="2"/>
-      <c r="D1388" s="2"/>
-    </row>
-    <row r="1423" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1423" s="2"/>
-      <c r="C1423" s="2"/>
-      <c r="D1423" s="2"/>
-    </row>
-    <row r="1424" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1424" s="2"/>
-      <c r="C1424" s="2"/>
-      <c r="D1424" s="2"/>
-    </row>
-    <row r="1425" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1425" s="2"/>
-      <c r="C1425" s="2"/>
-      <c r="D1425" s="2"/>
-    </row>
-    <row r="1426" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1426" s="2"/>
-      <c r="C1426" s="2"/>
-      <c r="D1426" s="2"/>
-    </row>
-    <row r="1427" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1427" s="2"/>
-      <c r="C1427" s="2"/>
-      <c r="D1427" s="2"/>
-    </row>
-    <row r="1428" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1428" s="2"/>
-      <c r="C1428" s="2"/>
-      <c r="D1428" s="2"/>
-    </row>
-    <row r="1470" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="F1470" s="2"/>
-      <c r="G1470" s="2"/>
-    </row>
-    <row r="1471" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E1471" s="10"/>
-      <c r="F1471" s="2"/>
-      <c r="G1471" s="2"/>
-    </row>
-    <row r="1472" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E1472" s="10"/>
-      <c r="F1472" s="2"/>
-      <c r="G1472" s="2"/>
-    </row>
-    <row r="1473" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E1473" s="10"/>
-      <c r="F1473" s="2"/>
-      <c r="G1473" s="2"/>
-    </row>
-    <row r="1474" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="F1474" s="2"/>
-      <c r="G1474" s="2"/>
-    </row>
-    <row r="1537" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1537" s="2"/>
-      <c r="C1537" s="2"/>
-      <c r="D1537" s="2"/>
-    </row>
-    <row r="1538" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1538" s="2"/>
-      <c r="C1538" s="2"/>
-      <c r="D1538" s="2"/>
-    </row>
-    <row r="1539" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1539" s="2"/>
-      <c r="C1539" s="2"/>
-      <c r="D1539" s="2"/>
-    </row>
-    <row r="1540" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1540" s="2"/>
-      <c r="C1540" s="2"/>
-      <c r="D1540" s="2"/>
+    <row r="1353" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1353" s="2"/>
+      <c r="C1353" s="2"/>
+      <c r="D1353" s="2"/>
+    </row>
+    <row r="1354" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1354" s="2"/>
+      <c r="C1354" s="2"/>
+      <c r="D1354" s="2"/>
+    </row>
+    <row r="1355" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1355" s="2"/>
+      <c r="C1355" s="2"/>
+      <c r="D1355" s="2"/>
+    </row>
+    <row r="1356" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1356" s="2"/>
+      <c r="C1356" s="2"/>
+      <c r="D1356" s="2"/>
+    </row>
+    <row r="1357" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1357" s="2"/>
+      <c r="C1357" s="2"/>
+      <c r="D1357" s="2"/>
+    </row>
+    <row r="1358" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1358" s="2"/>
+      <c r="C1358" s="2"/>
+      <c r="D1358" s="2"/>
+    </row>
+    <row r="1400" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F1400" s="2"/>
+      <c r="G1400" s="2"/>
+    </row>
+    <row r="1401" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1401" s="10"/>
+      <c r="F1401" s="2"/>
+      <c r="G1401" s="2"/>
+    </row>
+    <row r="1402" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1402" s="10"/>
+      <c r="F1402" s="2"/>
+      <c r="G1402" s="2"/>
+    </row>
+    <row r="1403" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E1403" s="10"/>
+      <c r="F1403" s="2"/>
+      <c r="G1403" s="2"/>
+    </row>
+    <row r="1404" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="F1404" s="2"/>
+      <c r="G1404" s="2"/>
+    </row>
+    <row r="1467" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1467" s="2"/>
+      <c r="C1467" s="2"/>
+      <c r="D1467" s="2"/>
+    </row>
+    <row r="1468" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1468" s="2"/>
+      <c r="C1468" s="2"/>
+      <c r="D1468" s="2"/>
+    </row>
+    <row r="1469" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1469" s="2"/>
+      <c r="C1469" s="2"/>
+      <c r="D1469" s="2"/>
+    </row>
+    <row r="1470" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1470" s="2"/>
+      <c r="C1470" s="2"/>
+      <c r="D1470" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G78">
-    <sortCondition ref="A4:A78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G8">
+    <sortCondition ref="A2:A8"/>
   </sortState>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -8028,6 +5975,251 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ACD7EE-6DEC-3B41-A0F3-0D49E6154785}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="6">
+        <v>1</v>
+      </c>
+      <c r="G1" s="6">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>153</v>
+      </c>
+      <c r="G2">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>1042</v>
+      </c>
+      <c r="G3">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="6">
+        <v>79</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1139</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2926</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="6">
+        <v>350</v>
+      </c>
+      <c r="G9">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1366</v>
+      </c>
+      <c r="G10">
+        <v>2874</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Validated Rep & Cap phylogeny build in genus Circo and Cyclo
</commit_message>
<xml_diff>
--- a/tabular/genus/cyclo_reference_feature_locations.xlsx
+++ b/tabular/genus/cyclo_reference_feature_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/genus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BE71D0-154F-A346-A46D-C4A622F73903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D40A40-CF13-1142-BBE5-A648CAB14672}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="31060" windowHeight="28340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,7 +140,7 @@
     <t>CBSV</t>
   </si>
   <si>
-    <t>REF_CRESS2_MASTER_Po-41</t>
+    <t>REF_MASTER_CRESS2_Po-41</t>
   </si>
 </sst>
 </file>
@@ -4762,7 +4762,7 @@
   <dimension ref="A1:G1470"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E8" sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>